<commit_message>
Class changes graphics, triggers,
Still need to finish the xp changes
</commit_message>
<xml_diff>
--- a/lvl calculation.xlsx
+++ b/lvl calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Paradox Interactive\Crusader Kings II\mod\faerun\Faerun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08DD3873-657A-4B41-9CAC-68FAF0E3F5BF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE9AA08-2FFD-475E-8057-1FC1FDC61B5E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17610" xr2:uid="{A142C3DE-DAF3-4A82-8F4A-DC9D72326703}"/>
   </bookViews>
@@ -22,6 +22,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,15 +375,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1887BC3E-7C42-4BE0-975A-3584B7959E05}">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -390,7 +394,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -402,7 +406,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -414,7 +418,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -426,7 +430,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>59</v>
       </c>
@@ -438,7 +442,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -450,7 +454,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -462,7 +466,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -473,8 +477,16 @@
       <c r="C8">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f>SUM(B8,B9,B10,B11,B12,B13,B14,B15,B16,B17,B18,B19,B20,B21,B22,B23,B24,B25,B26,B27,B28,B29,B30)</f>
+        <v>6200.2740675545738</v>
+      </c>
+      <c r="E8">
+        <f>(D8/25)</f>
+        <v>248.01096270218295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -486,7 +498,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -498,7 +510,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -510,7 +522,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -522,7 +534,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -534,7 +546,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -546,7 +558,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -558,7 +570,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -619,6 +631,9 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
       <c r="B21">
         <f t="shared" si="0"/>
         <v>269.09999797302441</v>
@@ -628,6 +643,9 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
       <c r="B22">
         <f t="shared" si="0"/>
         <v>296.00999777032689</v>
@@ -637,6 +655,9 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
       <c r="B23">
         <f t="shared" si="0"/>
         <v>325.6109975473596</v>
@@ -646,6 +667,9 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
       <c r="B24">
         <f t="shared" si="0"/>
         <v>358.17209730209561</v>
@@ -655,6 +679,9 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
       <c r="B25">
         <f t="shared" si="0"/>
         <v>393.98930703230519</v>
@@ -664,6 +691,9 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
       <c r="B26">
         <f t="shared" si="0"/>
         <v>433.38823773553577</v>
@@ -673,6 +703,9 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
       <c r="B27">
         <f t="shared" si="0"/>
         <v>476.72706150908937</v>
@@ -682,6 +715,9 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
       <c r="B28">
         <f t="shared" si="0"/>
         <v>524.39976765999836</v>
@@ -691,6 +727,9 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
       <c r="B29">
         <f t="shared" si="0"/>
         <v>576.83974442599822</v>
@@ -700,6 +739,9 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
       <c r="B30">
         <f t="shared" si="0"/>
         <v>634.52371886859805</v>
@@ -1034,7 +1076,7 @@
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67">
-        <f t="shared" ref="B67:B100" si="1">PRODUCT(B66,C66)</f>
+        <f t="shared" ref="B67:B99" si="1">PRODUCT(B66,C66)</f>
         <v>21576.311913105481</v>
       </c>
       <c r="C67">

</xml_diff>